<commit_message>
Added variables needed for changelogs
$changes added to store last changes actually made. Will need to store
old and new values of any other variable changed.
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Revision</t>
   </si>
   <si>
-    <t>Core/Customer/Catering</t>
-  </si>
-  <si>
     <t>Booking Price</t>
   </si>
   <si>
@@ -251,6 +248,15 @@
   </si>
   <si>
     <t>bLast</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>Changes Made</t>
+  </si>
+  <si>
+    <t>Core/Customer/Catering/Assets</t>
   </si>
 </sst>
 </file>
@@ -577,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" activeCellId="2" sqref="A16 A17 A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +594,7 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -607,7 +613,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -621,7 +627,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -635,7 +641,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -649,7 +655,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -663,7 +669,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -674,7 +680,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
@@ -688,7 +694,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
@@ -702,7 +708,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
@@ -716,7 +722,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
@@ -730,7 +736,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>43</v>
@@ -744,7 +750,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -758,7 +764,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
@@ -772,7 +778,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -786,7 +792,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
@@ -800,7 +806,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -814,7 +820,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
@@ -828,7 +834,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
@@ -842,7 +848,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -856,7 +862,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -870,7 +876,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
         <v>32</v>
@@ -884,7 +890,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
         <v>34</v>
@@ -898,7 +904,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
@@ -912,7 +918,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
@@ -926,7 +932,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
@@ -940,7 +946,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" t="s">
         <v>45</v>
@@ -949,15 +955,15 @@
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
         <v>33</v>
@@ -968,16 +974,30 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -988,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,54 +1033,57 @@
     <col min="16" max="16" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>53</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
       <c r="J1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" t="s">
         <v>61</v>
       </c>
-      <c r="L1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" t="s">
-        <v>62</v>
-      </c>
-      <c r="O1" t="s">
-        <v>63</v>
-      </c>
-      <c r="P1" t="s">
-        <v>70</v>
+      <c r="Q1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1070,10 +1093,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,27 +1109,30 @@
     <col min="7" max="7" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
         <v>73</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1116,10 +1142,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,15 +1155,18 @@
     <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1147,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,15 +1189,18 @@
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>